<commit_message>
update weighted edges codes
</commit_message>
<xml_diff>
--- a/European_electricity_network_vFinal.xlsx
+++ b/European_electricity_network_vFinal.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Sophie/Documents/02_Study/01_Programming_DataAnalysis/00_HSLU_MasterDataScience/00_Courses/07_AMS/Project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Sophie/Documents/GitHub/Analysis_and_Modelling_Social_Interactions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F8456D5-5264-5C4F-9218-31F5160C48CC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFFD0E66-4FAE-C04D-847E-3A00AEA1E2FE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38360" yWindow="460" windowWidth="29480" windowHeight="21100" xr2:uid="{FA1342EB-858C-E043-8F68-F0E6F5035E02}"/>
+    <workbookView xWindow="1900" yWindow="640" windowWidth="29480" windowHeight="21100" xr2:uid="{FA1342EB-858C-E043-8F68-F0E6F5035E02}"/>
   </bookViews>
   <sheets>
     <sheet name="2009" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="105">
   <si>
     <t>Albania</t>
   </si>
@@ -731,56 +731,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="37">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -1656,6 +1606,56 @@
       </fill>
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1670,44 +1670,44 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B0251C63-90C7-DE46-8BCB-D18A6BFAB1FC}" name="Table1" displayName="Table1" ref="C1:AK35" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
-  <autoFilter ref="C1:AK35" xr:uid="{E44B6400-29B5-B14A-B9F4-BFF4FA3220A3}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B0251C63-90C7-DE46-8BCB-D18A6BFAB1FC}" name="Table1" displayName="Table1" ref="B1:AJ35" totalsRowShown="0" headerRowDxfId="36" dataDxfId="35">
+  <autoFilter ref="B1:AJ35" xr:uid="{E44B6400-29B5-B14A-B9F4-BFF4FA3220A3}"/>
   <tableColumns count="35">
-    <tableColumn id="1" xr3:uid="{763C8FA9-BD8E-684F-9694-682B9C2EE09B}" name="Country_Code" dataDxfId="36"/>
-    <tableColumn id="2" xr3:uid="{5A360F38-6DD1-2E4B-95EA-A4284AB38C7C}" name="AL" dataDxfId="35"/>
-    <tableColumn id="3" xr3:uid="{6E44E9D3-A2EC-5545-8B1A-5DBEC4526D8D}" name="AT" dataDxfId="34"/>
-    <tableColumn id="4" xr3:uid="{9011CA24-C291-A147-8CD9-8179BF7C08D5}" name="BA" dataDxfId="33"/>
-    <tableColumn id="5" xr3:uid="{C03B5FB5-BFE8-164E-BF58-FC6C290C5157}" name="BE" dataDxfId="32"/>
-    <tableColumn id="6" xr3:uid="{914697DD-1920-B942-BA9E-6E2D0D2C5A1A}" name="BG" dataDxfId="31"/>
-    <tableColumn id="7" xr3:uid="{8B0F7679-DB0E-B745-8AB1-84C93BB6517C}" name="CH" dataDxfId="30"/>
-    <tableColumn id="8" xr3:uid="{5A7AEE85-2381-8542-9A69-5D3A47B0BEAD}" name="CZ" dataDxfId="29"/>
-    <tableColumn id="9" xr3:uid="{88A2FEA6-D60A-4F47-BA07-C658C684C937}" name="DE" dataDxfId="28"/>
-    <tableColumn id="10" xr3:uid="{24035C8E-464D-1644-AB91-137BFBA77482}" name="DK" dataDxfId="27"/>
-    <tableColumn id="11" xr3:uid="{3E15E16A-4BD6-5448-A19D-941C9B125DA4}" name="EE" dataDxfId="26"/>
-    <tableColumn id="12" xr3:uid="{4EC045FD-7454-A146-83CC-A5701527E126}" name="ES" dataDxfId="25"/>
-    <tableColumn id="13" xr3:uid="{6B138010-2D68-E548-92B8-C4BB2701A438}" name="FI" dataDxfId="24"/>
-    <tableColumn id="14" xr3:uid="{4EBB5515-47B5-494E-A421-F842E9C02D9C}" name="FR" dataDxfId="23"/>
-    <tableColumn id="15" xr3:uid="{2D8BDB26-3CF0-4642-83A6-DE5C40F91B96}" name="GB" dataDxfId="22"/>
-    <tableColumn id="16" xr3:uid="{FFD6276D-3A56-8B4B-893B-2938E819EEF8}" name="GR" dataDxfId="21"/>
-    <tableColumn id="17" xr3:uid="{67B64923-F9DA-F64A-B05C-7E39EAF554B2}" name="HR" dataDxfId="20"/>
-    <tableColumn id="18" xr3:uid="{8DFFC2F7-31CC-0747-B586-221E6DDC3773}" name="HU" dataDxfId="19"/>
-    <tableColumn id="19" xr3:uid="{9C2DC1BD-6239-4347-8102-E6FA046EFA6F}" name="IE" dataDxfId="18"/>
-    <tableColumn id="20" xr3:uid="{5840BD87-E8D8-FB47-89A7-2C9827EC7479}" name="IT" dataDxfId="17"/>
-    <tableColumn id="21" xr3:uid="{648F8721-D082-D049-8120-EE3E7720D140}" name="LT" dataDxfId="16"/>
-    <tableColumn id="22" xr3:uid="{F3708816-09D2-D24E-A5E2-A9C8D836BC17}" name="LU" dataDxfId="15"/>
-    <tableColumn id="23" xr3:uid="{048F84B4-5F5B-044B-BB79-70D609345F60}" name="LV" dataDxfId="14"/>
-    <tableColumn id="24" xr3:uid="{29A67122-9C40-604B-924E-60959D66D737}" name="ME" dataDxfId="13"/>
-    <tableColumn id="25" xr3:uid="{5919BBC8-5D22-1148-B40B-ED2DC205AF0E}" name="MK" dataDxfId="12"/>
-    <tableColumn id="26" xr3:uid="{5FE6528A-D997-6C48-9974-70A7F20935F4}" name="NL" dataDxfId="11"/>
-    <tableColumn id="27" xr3:uid="{EFD8C00E-704D-4D4A-A280-4B43F4FE3E7C}" name="NO" dataDxfId="10"/>
-    <tableColumn id="28" xr3:uid="{2D83C8B5-C901-0A4E-B261-FB766E027E81}" name="PL" dataDxfId="9"/>
-    <tableColumn id="29" xr3:uid="{C79A3262-F4B4-5A4F-8960-F4B152AA0844}" name="PT" dataDxfId="8"/>
-    <tableColumn id="30" xr3:uid="{01576C2D-FEC5-324A-B907-90C09277D52D}" name="RO" dataDxfId="7"/>
-    <tableColumn id="31" xr3:uid="{01901CF5-2491-F043-9BDF-2C7138540FE8}" name="RS" dataDxfId="6"/>
-    <tableColumn id="32" xr3:uid="{8B3C1362-5862-414F-9148-66638F05CCBB}" name="SE" dataDxfId="5"/>
-    <tableColumn id="33" xr3:uid="{C76BA514-86E5-374D-A69C-6AC29EA84F60}" name="SI" dataDxfId="4"/>
-    <tableColumn id="34" xr3:uid="{4BB7C62E-B28C-F847-A6E7-8FC4B32CF40E}" name="SK" dataDxfId="3"/>
-    <tableColumn id="35" xr3:uid="{9F9D515F-0B1C-B543-A5EA-63547B79068D}" name="TR" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{763C8FA9-BD8E-684F-9694-682B9C2EE09B}" name="Country_Code" dataDxfId="34"/>
+    <tableColumn id="2" xr3:uid="{5A360F38-6DD1-2E4B-95EA-A4284AB38C7C}" name="AL" dataDxfId="33"/>
+    <tableColumn id="3" xr3:uid="{6E44E9D3-A2EC-5545-8B1A-5DBEC4526D8D}" name="AT" dataDxfId="32"/>
+    <tableColumn id="4" xr3:uid="{9011CA24-C291-A147-8CD9-8179BF7C08D5}" name="BA" dataDxfId="31"/>
+    <tableColumn id="5" xr3:uid="{C03B5FB5-BFE8-164E-BF58-FC6C290C5157}" name="BE" dataDxfId="30"/>
+    <tableColumn id="6" xr3:uid="{914697DD-1920-B942-BA9E-6E2D0D2C5A1A}" name="BG" dataDxfId="29"/>
+    <tableColumn id="7" xr3:uid="{8B0F7679-DB0E-B745-8AB1-84C93BB6517C}" name="CH" dataDxfId="28"/>
+    <tableColumn id="8" xr3:uid="{5A7AEE85-2381-8542-9A69-5D3A47B0BEAD}" name="CZ" dataDxfId="27"/>
+    <tableColumn id="9" xr3:uid="{88A2FEA6-D60A-4F47-BA07-C658C684C937}" name="DE" dataDxfId="26"/>
+    <tableColumn id="10" xr3:uid="{24035C8E-464D-1644-AB91-137BFBA77482}" name="DK" dataDxfId="25"/>
+    <tableColumn id="11" xr3:uid="{3E15E16A-4BD6-5448-A19D-941C9B125DA4}" name="EE" dataDxfId="24"/>
+    <tableColumn id="12" xr3:uid="{4EC045FD-7454-A146-83CC-A5701527E126}" name="ES" dataDxfId="23"/>
+    <tableColumn id="13" xr3:uid="{6B138010-2D68-E548-92B8-C4BB2701A438}" name="FI" dataDxfId="22"/>
+    <tableColumn id="14" xr3:uid="{4EBB5515-47B5-494E-A421-F842E9C02D9C}" name="FR" dataDxfId="21"/>
+    <tableColumn id="15" xr3:uid="{2D8BDB26-3CF0-4642-83A6-DE5C40F91B96}" name="GB" dataDxfId="20"/>
+    <tableColumn id="16" xr3:uid="{FFD6276D-3A56-8B4B-893B-2938E819EEF8}" name="GR" dataDxfId="19"/>
+    <tableColumn id="17" xr3:uid="{67B64923-F9DA-F64A-B05C-7E39EAF554B2}" name="HR" dataDxfId="18"/>
+    <tableColumn id="18" xr3:uid="{8DFFC2F7-31CC-0747-B586-221E6DDC3773}" name="HU" dataDxfId="17"/>
+    <tableColumn id="19" xr3:uid="{9C2DC1BD-6239-4347-8102-E6FA046EFA6F}" name="IE" dataDxfId="16"/>
+    <tableColumn id="20" xr3:uid="{5840BD87-E8D8-FB47-89A7-2C9827EC7479}" name="IT" dataDxfId="15"/>
+    <tableColumn id="21" xr3:uid="{648F8721-D082-D049-8120-EE3E7720D140}" name="LT" dataDxfId="14"/>
+    <tableColumn id="22" xr3:uid="{F3708816-09D2-D24E-A5E2-A9C8D836BC17}" name="LU" dataDxfId="13"/>
+    <tableColumn id="23" xr3:uid="{048F84B4-5F5B-044B-BB79-70D609345F60}" name="LV" dataDxfId="12"/>
+    <tableColumn id="24" xr3:uid="{29A67122-9C40-604B-924E-60959D66D737}" name="ME" dataDxfId="11"/>
+    <tableColumn id="25" xr3:uid="{5919BBC8-5D22-1148-B40B-ED2DC205AF0E}" name="MK" dataDxfId="10"/>
+    <tableColumn id="26" xr3:uid="{5FE6528A-D997-6C48-9974-70A7F20935F4}" name="NL" dataDxfId="9"/>
+    <tableColumn id="27" xr3:uid="{EFD8C00E-704D-4D4A-A280-4B43F4FE3E7C}" name="NO" dataDxfId="8"/>
+    <tableColumn id="28" xr3:uid="{2D83C8B5-C901-0A4E-B261-FB766E027E81}" name="PL" dataDxfId="7"/>
+    <tableColumn id="29" xr3:uid="{C79A3262-F4B4-5A4F-8960-F4B152AA0844}" name="PT" dataDxfId="6"/>
+    <tableColumn id="30" xr3:uid="{01576C2D-FEC5-324A-B907-90C09277D52D}" name="RO" dataDxfId="5"/>
+    <tableColumn id="31" xr3:uid="{01901CF5-2491-F043-9BDF-2C7138540FE8}" name="RS" dataDxfId="4"/>
+    <tableColumn id="32" xr3:uid="{8B3C1362-5862-414F-9148-66638F05CCBB}" name="SE" dataDxfId="3"/>
+    <tableColumn id="33" xr3:uid="{C76BA514-86E5-374D-A69C-6AC29EA84F60}" name="SI" dataDxfId="2"/>
+    <tableColumn id="34" xr3:uid="{4BB7C62E-B28C-F847-A6E7-8FC4B32CF40E}" name="SK" dataDxfId="1"/>
+    <tableColumn id="35" xr3:uid="{9F9D515F-0B1C-B543-A5EA-63547B79068D}" name="TR" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2010,295 +2010,288 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{095C5849-7156-4148-91CA-BD8F3296F257}">
-  <dimension ref="A1:AK35"/>
+  <dimension ref="A1:AJ35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="90" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G16" sqref="G16"/>
+      <selection pane="bottomLeft" activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="7.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13.5" style="3" customWidth="1"/>
-    <col min="2" max="2" width="20.83203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.83203125" style="3" customWidth="1"/>
-    <col min="4" max="4" width="7" style="3" customWidth="1"/>
-    <col min="5" max="5" width="7.1640625" style="3" customWidth="1"/>
-    <col min="6" max="6" width="7.33203125" style="3" customWidth="1"/>
-    <col min="7" max="7" width="7.1640625" style="3" customWidth="1"/>
-    <col min="8" max="8" width="7.5" style="3" customWidth="1"/>
-    <col min="9" max="9" width="7.1640625" style="3" customWidth="1"/>
-    <col min="10" max="10" width="7" style="3" customWidth="1"/>
-    <col min="11" max="12" width="7.1640625" style="3" customWidth="1"/>
-    <col min="13" max="14" width="7" style="3" customWidth="1"/>
-    <col min="15" max="15" width="6.5" style="3" customWidth="1"/>
-    <col min="16" max="16" width="7.1640625" style="3" customWidth="1"/>
-    <col min="17" max="18" width="7.5" style="3" customWidth="1"/>
-    <col min="19" max="19" width="7.33203125" style="3" customWidth="1"/>
-    <col min="20" max="20" width="7.5" style="3" customWidth="1"/>
-    <col min="21" max="21" width="6.5" style="3" customWidth="1"/>
-    <col min="22" max="22" width="6.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="6.83203125" style="3" customWidth="1"/>
-    <col min="24" max="24" width="7.1640625" style="3" customWidth="1"/>
-    <col min="25" max="25" width="7" style="3" customWidth="1"/>
-    <col min="26" max="27" width="7.6640625" style="3" customWidth="1"/>
-    <col min="28" max="28" width="7.1640625" style="3" customWidth="1"/>
-    <col min="29" max="29" width="7.6640625" style="3" customWidth="1"/>
-    <col min="30" max="30" width="6.83203125" style="3" customWidth="1"/>
-    <col min="31" max="31" width="7" style="3" customWidth="1"/>
-    <col min="32" max="32" width="7.5" style="3" customWidth="1"/>
-    <col min="33" max="33" width="7.1640625" style="3" customWidth="1"/>
-    <col min="34" max="34" width="7" style="3" customWidth="1"/>
-    <col min="35" max="35" width="6.5" style="3" customWidth="1"/>
-    <col min="36" max="36" width="7" style="3" customWidth="1"/>
-    <col min="37" max="37" width="7.1640625" style="3" customWidth="1"/>
-    <col min="38" max="38" width="5.83203125" style="3" customWidth="1"/>
-    <col min="39" max="39" width="6.33203125" style="3" customWidth="1"/>
-    <col min="40" max="16384" width="7.5" style="3"/>
+    <col min="2" max="2" width="7.83203125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="7" style="3" customWidth="1"/>
+    <col min="4" max="4" width="7.1640625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="7.33203125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="7.1640625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="7.5" style="3" customWidth="1"/>
+    <col min="8" max="8" width="7.1640625" style="3" customWidth="1"/>
+    <col min="9" max="9" width="7" style="3" customWidth="1"/>
+    <col min="10" max="11" width="7.1640625" style="3" customWidth="1"/>
+    <col min="12" max="13" width="7" style="3" customWidth="1"/>
+    <col min="14" max="14" width="6.5" style="3" customWidth="1"/>
+    <col min="15" max="15" width="7.1640625" style="3" customWidth="1"/>
+    <col min="16" max="17" width="7.5" style="3" customWidth="1"/>
+    <col min="18" max="18" width="7.33203125" style="3" customWidth="1"/>
+    <col min="19" max="19" width="7.5" style="3" customWidth="1"/>
+    <col min="20" max="20" width="6.5" style="3" customWidth="1"/>
+    <col min="21" max="21" width="6.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="6.83203125" style="3" customWidth="1"/>
+    <col min="23" max="23" width="7.1640625" style="3" customWidth="1"/>
+    <col min="24" max="24" width="7" style="3" customWidth="1"/>
+    <col min="25" max="26" width="7.6640625" style="3" customWidth="1"/>
+    <col min="27" max="27" width="7.1640625" style="3" customWidth="1"/>
+    <col min="28" max="28" width="7.6640625" style="3" customWidth="1"/>
+    <col min="29" max="29" width="6.83203125" style="3" customWidth="1"/>
+    <col min="30" max="30" width="7" style="3" customWidth="1"/>
+    <col min="31" max="31" width="7.5" style="3" customWidth="1"/>
+    <col min="32" max="32" width="7.1640625" style="3" customWidth="1"/>
+    <col min="33" max="33" width="7" style="3" customWidth="1"/>
+    <col min="34" max="34" width="6.5" style="3" customWidth="1"/>
+    <col min="35" max="35" width="7" style="3" customWidth="1"/>
+    <col min="36" max="36" width="7.1640625" style="3" customWidth="1"/>
+    <col min="37" max="37" width="5.83203125" style="3" customWidth="1"/>
+    <col min="38" max="38" width="6.33203125" style="3" customWidth="1"/>
+    <col min="39" max="16384" width="7.5" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:36" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="C1" s="4" t="s">
+      <c r="B1" s="4" t="s">
         <v>70</v>
       </c>
+      <c r="C1" s="7" t="s">
+        <v>72</v>
+      </c>
       <c r="D1" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="J1" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="K1" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="L1" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="M1" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="N1" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="O1" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="P1" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q1" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="R1" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="S1" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="T1" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="U1" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="V1" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="W1" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="X1" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="Y1" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="Z1" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="AA1" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="AB1" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="AC1" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="AD1" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="AE1" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="AF1" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="AG1" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="AH1" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="AI1" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="AJ1" s="7" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="2" spans="1:36" ht="17" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="E1" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="F1" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="G1" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="H1" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="I1" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="J1" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="K1" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="L1" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="M1" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="N1" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="O1" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="P1" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="Q1" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="R1" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="S1" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="T1" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="U1" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="V1" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="W1" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="X1" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="Y1" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="Z1" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="AA1" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="AB1" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="AC1" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="AD1" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="AE1" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="AF1" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="AG1" s="7" t="s">
-        <v>100</v>
-      </c>
-      <c r="AH1" s="7" t="s">
-        <v>101</v>
-      </c>
-      <c r="AI1" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="AJ1" s="7" t="s">
-        <v>103</v>
-      </c>
-      <c r="AK1" s="7" t="s">
-        <v>104</v>
+      <c r="C2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="3">
+        <v>0</v>
+      </c>
+      <c r="E2" s="3">
+        <v>0</v>
+      </c>
+      <c r="F2" s="3">
+        <v>0</v>
+      </c>
+      <c r="G2" s="3">
+        <v>0</v>
+      </c>
+      <c r="H2" s="3">
+        <v>0</v>
+      </c>
+      <c r="I2" s="3">
+        <v>0</v>
+      </c>
+      <c r="J2" s="3">
+        <v>0</v>
+      </c>
+      <c r="K2" s="3">
+        <v>0</v>
+      </c>
+      <c r="L2" s="3">
+        <v>0</v>
+      </c>
+      <c r="M2" s="3">
+        <v>0</v>
+      </c>
+      <c r="N2" s="3">
+        <v>0</v>
+      </c>
+      <c r="O2" s="3">
+        <v>0</v>
+      </c>
+      <c r="P2" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="3">
+        <v>61</v>
+      </c>
+      <c r="R2" s="3">
+        <v>0</v>
+      </c>
+      <c r="S2" s="3">
+        <v>0</v>
+      </c>
+      <c r="T2" s="3">
+        <v>0</v>
+      </c>
+      <c r="U2" s="3">
+        <v>0</v>
+      </c>
+      <c r="V2" s="3">
+        <v>0</v>
+      </c>
+      <c r="W2" s="3">
+        <v>0</v>
+      </c>
+      <c r="X2" s="3">
+        <v>0</v>
+      </c>
+      <c r="Y2" s="3">
+        <v>47</v>
+      </c>
+      <c r="Z2" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA2" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB2" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC2" s="3">
+        <v>0</v>
+      </c>
+      <c r="AD2" s="3">
+        <v>0</v>
+      </c>
+      <c r="AE2" s="3">
+        <v>0</v>
+      </c>
+      <c r="AF2" s="3">
+        <v>425</v>
+      </c>
+      <c r="AG2" s="3">
+        <v>0</v>
+      </c>
+      <c r="AH2" s="3">
+        <v>0</v>
+      </c>
+      <c r="AI2" s="3">
+        <v>0</v>
+      </c>
+      <c r="AJ2" s="3">
+        <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:37" ht="17" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2" s="3">
-        <v>0</v>
-      </c>
-      <c r="F2" s="3">
-        <v>0</v>
-      </c>
-      <c r="G2" s="3">
-        <v>0</v>
-      </c>
-      <c r="H2" s="3">
-        <v>0</v>
-      </c>
-      <c r="I2" s="3">
-        <v>0</v>
-      </c>
-      <c r="J2" s="3">
-        <v>0</v>
-      </c>
-      <c r="K2" s="3">
-        <v>0</v>
-      </c>
-      <c r="L2" s="3">
-        <v>0</v>
-      </c>
-      <c r="M2" s="3">
-        <v>0</v>
-      </c>
-      <c r="N2" s="3">
-        <v>0</v>
-      </c>
-      <c r="O2" s="3">
-        <v>0</v>
-      </c>
-      <c r="P2" s="3">
-        <v>0</v>
-      </c>
-      <c r="Q2" s="3">
-        <v>0</v>
-      </c>
-      <c r="R2" s="3">
-        <v>61</v>
-      </c>
-      <c r="S2" s="3">
-        <v>0</v>
-      </c>
-      <c r="T2" s="3">
-        <v>0</v>
-      </c>
-      <c r="U2" s="3">
-        <v>0</v>
-      </c>
-      <c r="V2" s="3">
-        <v>0</v>
-      </c>
-      <c r="W2" s="3">
-        <v>0</v>
-      </c>
-      <c r="X2" s="3">
-        <v>0</v>
-      </c>
-      <c r="Y2" s="3">
-        <v>0</v>
-      </c>
-      <c r="Z2" s="3">
-        <v>47</v>
-      </c>
-      <c r="AA2" s="3">
-        <v>0</v>
-      </c>
-      <c r="AB2" s="3">
-        <v>0</v>
-      </c>
-      <c r="AC2" s="3">
-        <v>0</v>
-      </c>
-      <c r="AD2" s="3">
-        <v>0</v>
-      </c>
-      <c r="AE2" s="3">
-        <v>0</v>
-      </c>
-      <c r="AF2" s="3">
-        <v>0</v>
-      </c>
-      <c r="AG2" s="3">
-        <v>425</v>
-      </c>
-      <c r="AH2" s="3">
-        <v>0</v>
-      </c>
-      <c r="AI2" s="3">
-        <v>0</v>
-      </c>
-      <c r="AJ2" s="3">
-        <v>0</v>
-      </c>
-      <c r="AK2" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:37" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:36" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="7" t="s">
+      <c r="B3" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="D3" s="3">
-        <v>0</v>
-      </c>
-      <c r="E3" s="3" t="s">
+      <c r="C3" s="3">
+        <v>0</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>1</v>
       </c>
+      <c r="E3" s="3">
+        <v>0</v>
+      </c>
       <c r="F3" s="3">
         <v>0</v>
       </c>
@@ -2306,16 +2299,16 @@
         <v>0</v>
       </c>
       <c r="H3" s="3">
-        <v>0</v>
+        <v>8653</v>
       </c>
       <c r="I3" s="3">
-        <v>8653</v>
+        <v>262</v>
       </c>
       <c r="J3" s="3">
-        <v>262</v>
+        <v>7061</v>
       </c>
       <c r="K3" s="3">
-        <v>7061</v>
+        <v>0</v>
       </c>
       <c r="L3" s="3">
         <v>0</v>
@@ -2339,16 +2332,16 @@
         <v>0</v>
       </c>
       <c r="S3" s="3">
-        <v>0</v>
+        <v>1393</v>
       </c>
       <c r="T3" s="3">
-        <v>1393</v>
+        <v>0</v>
       </c>
       <c r="U3" s="3">
-        <v>0</v>
+        <v>1198</v>
       </c>
       <c r="V3" s="3">
-        <v>1198</v>
+        <v>0</v>
       </c>
       <c r="W3" s="3">
         <v>0</v>
@@ -2384,37 +2377,34 @@
         <v>0</v>
       </c>
       <c r="AH3" s="3">
-        <v>0</v>
+        <v>2527</v>
       </c>
       <c r="AI3" s="3">
-        <v>2527</v>
+        <v>0</v>
       </c>
       <c r="AJ3" s="3">
         <v>0</v>
       </c>
-      <c r="AK3" s="3">
-        <v>0</v>
-      </c>
     </row>
-    <row r="4" spans="1:37" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:36" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="7" t="s">
+      <c r="B4" s="7" t="s">
         <v>74</v>
       </c>
+      <c r="C4" s="3">
+        <v>0</v>
+      </c>
       <c r="D4" s="3">
         <v>0</v>
       </c>
-      <c r="E4" s="3">
-        <v>0</v>
-      </c>
-      <c r="F4" s="3" t="s">
+      <c r="E4" s="3" t="s">
         <v>1</v>
       </c>
+      <c r="F4" s="3">
+        <v>0</v>
+      </c>
       <c r="G4" s="3">
         <v>0</v>
       </c>
@@ -2449,10 +2439,10 @@
         <v>0</v>
       </c>
       <c r="R4" s="3">
-        <v>0</v>
+        <v>3280</v>
       </c>
       <c r="S4" s="3">
-        <v>3280</v>
+        <v>0</v>
       </c>
       <c r="T4" s="3">
         <v>0</v>
@@ -2470,10 +2460,10 @@
         <v>0</v>
       </c>
       <c r="Y4" s="3">
-        <v>0</v>
+        <v>2195</v>
       </c>
       <c r="Z4" s="3">
-        <v>2195</v>
+        <v>0</v>
       </c>
       <c r="AA4" s="3">
         <v>0</v>
@@ -2491,10 +2481,10 @@
         <v>0</v>
       </c>
       <c r="AF4" s="3">
-        <v>0</v>
+        <v>361</v>
       </c>
       <c r="AG4" s="3">
-        <v>361</v>
+        <v>0</v>
       </c>
       <c r="AH4" s="3">
         <v>0</v>
@@ -2505,32 +2495,29 @@
       <c r="AJ4" s="3">
         <v>0</v>
       </c>
-      <c r="AK4" s="3">
-        <v>0</v>
-      </c>
     </row>
-    <row r="5" spans="1:37" ht="17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:36" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" s="7" t="s">
+      <c r="B5" s="7" t="s">
         <v>75</v>
       </c>
+      <c r="C5" s="3">
+        <v>0</v>
+      </c>
       <c r="D5" s="3">
         <v>0</v>
       </c>
       <c r="E5" s="3">
         <v>0</v>
       </c>
-      <c r="F5" s="3">
-        <v>0</v>
-      </c>
-      <c r="G5" s="3" t="s">
+      <c r="F5" s="3" t="s">
         <v>1</v>
       </c>
+      <c r="G5" s="3">
+        <v>0</v>
+      </c>
       <c r="H5" s="3">
         <v>0</v>
       </c>
@@ -2553,10 +2540,10 @@
         <v>0</v>
       </c>
       <c r="O5" s="3">
-        <v>0</v>
+        <v>6630</v>
       </c>
       <c r="P5" s="3">
-        <v>6630</v>
+        <v>0</v>
       </c>
       <c r="Q5" s="3">
         <v>0</v>
@@ -2577,10 +2564,10 @@
         <v>0</v>
       </c>
       <c r="W5" s="3">
-        <v>0</v>
+        <v>911</v>
       </c>
       <c r="X5" s="3">
-        <v>911</v>
+        <v>0</v>
       </c>
       <c r="Y5" s="3">
         <v>0</v>
@@ -2589,10 +2576,10 @@
         <v>0</v>
       </c>
       <c r="AA5" s="3">
-        <v>0</v>
+        <v>3773</v>
       </c>
       <c r="AB5" s="3">
-        <v>3773</v>
+        <v>0</v>
       </c>
       <c r="AC5" s="3">
         <v>0</v>
@@ -2618,20 +2605,17 @@
       <c r="AJ5" s="3">
         <v>0</v>
       </c>
-      <c r="AK5" s="3">
-        <v>0</v>
-      </c>
     </row>
-    <row r="6" spans="1:37" ht="17" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:36" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="7" t="s">
+      <c r="B6" s="7" t="s">
         <v>76</v>
       </c>
+      <c r="C6" s="3">
+        <v>0</v>
+      </c>
       <c r="D6" s="3">
         <v>0</v>
       </c>
@@ -2641,12 +2625,12 @@
       <c r="F6" s="3">
         <v>0</v>
       </c>
-      <c r="G6" s="3">
-        <v>0</v>
-      </c>
-      <c r="H6" s="3" t="s">
+      <c r="G6" s="3" t="s">
         <v>1</v>
       </c>
+      <c r="H6" s="3">
+        <v>0</v>
+      </c>
       <c r="I6" s="3">
         <v>0</v>
       </c>
@@ -2672,10 +2656,10 @@
         <v>0</v>
       </c>
       <c r="Q6" s="3">
-        <v>0</v>
+        <v>3418</v>
       </c>
       <c r="R6" s="3">
-        <v>3418</v>
+        <v>0</v>
       </c>
       <c r="S6" s="3">
         <v>0</v>
@@ -2699,10 +2683,10 @@
         <v>0</v>
       </c>
       <c r="Z6" s="3">
-        <v>0</v>
+        <v>2802</v>
       </c>
       <c r="AA6" s="3">
-        <v>2802</v>
+        <v>0</v>
       </c>
       <c r="AB6" s="3">
         <v>0</v>
@@ -2714,13 +2698,13 @@
         <v>0</v>
       </c>
       <c r="AE6" s="3">
-        <v>0</v>
+        <v>230</v>
       </c>
       <c r="AF6" s="3">
-        <v>230</v>
+        <v>1184</v>
       </c>
       <c r="AG6" s="3">
-        <v>1184</v>
+        <v>0</v>
       </c>
       <c r="AH6" s="3">
         <v>0</v>
@@ -2731,25 +2715,22 @@
       <c r="AJ6" s="3">
         <v>0</v>
       </c>
-      <c r="AK6" s="3">
-        <v>0</v>
-      </c>
     </row>
-    <row r="7" spans="1:37" ht="17" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:36" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" s="7" t="s">
+      <c r="B7" s="7" t="s">
         <v>77</v>
       </c>
+      <c r="C7" s="3">
+        <v>0</v>
+      </c>
       <c r="D7" s="3">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="E7" s="3">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="F7" s="3">
         <v>0</v>
@@ -2757,17 +2738,17 @@
       <c r="G7" s="3">
         <v>0</v>
       </c>
-      <c r="H7" s="3">
-        <v>0</v>
-      </c>
-      <c r="I7" s="3" t="s">
+      <c r="H7" s="3" t="s">
         <v>1</v>
       </c>
+      <c r="I7" s="3">
+        <v>0</v>
+      </c>
       <c r="J7" s="3">
-        <v>0</v>
+        <v>2636</v>
       </c>
       <c r="K7" s="3">
-        <v>2636</v>
+        <v>0</v>
       </c>
       <c r="L7" s="3">
         <v>0</v>
@@ -2779,10 +2760,10 @@
         <v>0</v>
       </c>
       <c r="O7" s="3">
-        <v>0</v>
+        <v>4164</v>
       </c>
       <c r="P7" s="3">
-        <v>4164</v>
+        <v>0</v>
       </c>
       <c r="Q7" s="3">
         <v>0</v>
@@ -2797,10 +2778,10 @@
         <v>0</v>
       </c>
       <c r="U7" s="3">
-        <v>0</v>
+        <v>24958</v>
       </c>
       <c r="V7" s="3">
-        <v>24958</v>
+        <v>0</v>
       </c>
       <c r="W7" s="3">
         <v>0</v>
@@ -2844,25 +2825,22 @@
       <c r="AJ7" s="3">
         <v>0</v>
       </c>
-      <c r="AK7" s="3">
-        <v>0</v>
-      </c>
     </row>
-    <row r="8" spans="1:37" ht="17" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:36" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" s="7" t="s">
+      <c r="B8" s="7" t="s">
         <v>78</v>
       </c>
+      <c r="C8" s="3">
+        <v>0</v>
+      </c>
       <c r="D8" s="3">
-        <v>0</v>
+        <v>6859</v>
       </c>
       <c r="E8" s="3">
-        <v>6859</v>
+        <v>0</v>
       </c>
       <c r="F8" s="3">
         <v>0</v>
@@ -2873,14 +2851,14 @@
       <c r="H8" s="3">
         <v>0</v>
       </c>
-      <c r="I8" s="3">
-        <v>0</v>
-      </c>
-      <c r="J8" s="3" t="s">
+      <c r="I8" s="3" t="s">
         <v>1</v>
       </c>
+      <c r="J8" s="3">
+        <v>8687</v>
+      </c>
       <c r="K8" s="3">
-        <v>8687</v>
+        <v>0</v>
       </c>
       <c r="L8" s="3">
         <v>0</v>
@@ -2934,10 +2912,10 @@
         <v>0</v>
       </c>
       <c r="AC8" s="3">
-        <v>0</v>
+        <v>129</v>
       </c>
       <c r="AD8" s="3">
-        <v>129</v>
+        <v>0</v>
       </c>
       <c r="AE8" s="3">
         <v>0</v>
@@ -2952,30 +2930,27 @@
         <v>0</v>
       </c>
       <c r="AI8" s="3">
-        <v>0</v>
+        <v>6557</v>
       </c>
       <c r="AJ8" s="3">
-        <v>6557</v>
-      </c>
-      <c r="AK8" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:37" ht="17" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:36" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9" s="7" t="s">
+      <c r="B9" s="7" t="s">
         <v>79</v>
       </c>
+      <c r="C9" s="3">
+        <v>0</v>
+      </c>
       <c r="D9" s="3">
-        <v>0</v>
+        <v>14956</v>
       </c>
       <c r="E9" s="3">
-        <v>14956</v>
+        <v>0</v>
       </c>
       <c r="F9" s="3">
         <v>0</v>
@@ -2984,21 +2959,21 @@
         <v>0</v>
       </c>
       <c r="H9" s="3">
-        <v>0</v>
+        <v>13142</v>
       </c>
       <c r="I9" s="3">
-        <v>13142</v>
-      </c>
-      <c r="J9" s="3">
         <v>965</v>
       </c>
-      <c r="K9" s="3" t="s">
+      <c r="J9" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="L9" s="3">
+      <c r="K9" s="3">
         <f>1814+1801</f>
         <v>3615</v>
       </c>
+      <c r="L9" s="3">
+        <v>0</v>
+      </c>
       <c r="M9" s="3">
         <v>0</v>
       </c>
@@ -3006,10 +2981,10 @@
         <v>0</v>
       </c>
       <c r="O9" s="3">
-        <v>0</v>
+        <v>1436</v>
       </c>
       <c r="P9" s="3">
-        <v>1436</v>
+        <v>0</v>
       </c>
       <c r="Q9" s="3">
         <v>0</v>
@@ -3030,10 +3005,10 @@
         <v>0</v>
       </c>
       <c r="W9" s="3">
-        <v>0</v>
+        <v>5115</v>
       </c>
       <c r="X9" s="3">
-        <v>5115</v>
+        <v>0</v>
       </c>
       <c r="Y9" s="3">
         <v>0</v>
@@ -3042,16 +3017,16 @@
         <v>0</v>
       </c>
       <c r="AA9" s="3">
-        <v>0</v>
+        <v>8870</v>
       </c>
       <c r="AB9" s="3">
-        <v>8870</v>
+        <v>0</v>
       </c>
       <c r="AC9" s="3">
-        <v>0</v>
+        <v>5618</v>
       </c>
       <c r="AD9" s="3">
-        <v>5618</v>
+        <v>0</v>
       </c>
       <c r="AE9" s="3">
         <v>0</v>
@@ -3060,10 +3035,10 @@
         <v>0</v>
       </c>
       <c r="AG9" s="3">
-        <v>0</v>
+        <v>1132</v>
       </c>
       <c r="AH9" s="3">
-        <v>1132</v>
+        <v>0</v>
       </c>
       <c r="AI9" s="3">
         <v>0</v>
@@ -3071,20 +3046,17 @@
       <c r="AJ9" s="3">
         <v>0</v>
       </c>
-      <c r="AK9" s="3">
-        <v>0</v>
-      </c>
     </row>
-    <row r="10" spans="1:37" ht="17" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:36" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" s="7" t="s">
+      <c r="B10" s="7" t="s">
         <v>80</v>
       </c>
+      <c r="C10" s="3">
+        <v>0</v>
+      </c>
       <c r="D10" s="3">
         <v>0</v>
       </c>
@@ -3104,15 +3076,15 @@
         <v>0</v>
       </c>
       <c r="J10" s="3">
-        <v>0</v>
-      </c>
-      <c r="K10" s="3">
         <f>4946+1286</f>
         <v>6232</v>
       </c>
-      <c r="L10" s="3" t="s">
+      <c r="K10" s="3" t="s">
         <v>1</v>
       </c>
+      <c r="L10" s="3">
+        <v>0</v>
+      </c>
       <c r="M10" s="3">
         <v>0</v>
       </c>
@@ -3159,10 +3131,10 @@
         <v>0</v>
       </c>
       <c r="AB10" s="3">
-        <v>0</v>
+        <v>1448</v>
       </c>
       <c r="AC10" s="3">
-        <v>1448</v>
+        <v>0</v>
       </c>
       <c r="AD10" s="3">
         <v>0</v>
@@ -3174,10 +3146,10 @@
         <v>0</v>
       </c>
       <c r="AG10" s="3">
-        <v>0</v>
+        <v>3150</v>
       </c>
       <c r="AH10" s="3">
-        <v>3150</v>
+        <v>0</v>
       </c>
       <c r="AI10" s="3">
         <v>0</v>
@@ -3185,20 +3157,17 @@
       <c r="AJ10" s="3">
         <v>0</v>
       </c>
-      <c r="AK10" s="3">
-        <v>0</v>
-      </c>
     </row>
-    <row r="11" spans="1:37" ht="17" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:36" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C11" s="7" t="s">
+      <c r="B11" s="7" t="s">
         <v>81</v>
       </c>
+      <c r="C11" s="3">
+        <v>0</v>
+      </c>
       <c r="D11" s="3">
         <v>0</v>
       </c>
@@ -3223,17 +3192,17 @@
       <c r="K11" s="3">
         <v>0</v>
       </c>
-      <c r="L11" s="3">
-        <v>0</v>
-      </c>
-      <c r="M11" s="3" t="s">
+      <c r="L11" s="3" t="s">
         <v>1</v>
       </c>
+      <c r="M11" s="3">
+        <v>0</v>
+      </c>
       <c r="N11" s="3">
-        <v>0</v>
+        <v>1785</v>
       </c>
       <c r="O11" s="3">
-        <v>1785</v>
+        <v>0</v>
       </c>
       <c r="P11" s="3">
         <v>0</v>
@@ -3260,10 +3229,10 @@
         <v>0</v>
       </c>
       <c r="X11" s="3">
-        <v>0</v>
+        <v>1138</v>
       </c>
       <c r="Y11" s="3">
-        <v>1138</v>
+        <v>0</v>
       </c>
       <c r="Z11" s="3">
         <v>0</v>
@@ -3298,20 +3267,17 @@
       <c r="AJ11" s="3">
         <v>0</v>
       </c>
-      <c r="AK11" s="3">
-        <v>0</v>
-      </c>
     </row>
-    <row r="12" spans="1:37" ht="17" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:36" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C12" s="7" t="s">
+      <c r="B12" s="7" t="s">
         <v>82</v>
       </c>
+      <c r="C12" s="3">
+        <v>0</v>
+      </c>
       <c r="D12" s="3">
         <v>0</v>
       </c>
@@ -3339,17 +3305,17 @@
       <c r="L12" s="3">
         <v>0</v>
       </c>
-      <c r="M12" s="3">
-        <v>0</v>
-      </c>
-      <c r="N12" s="3" t="s">
+      <c r="M12" s="3" t="s">
         <v>1</v>
       </c>
+      <c r="N12" s="3">
+        <v>0</v>
+      </c>
       <c r="O12" s="3">
-        <v>0</v>
+        <v>2351</v>
       </c>
       <c r="P12" s="3">
-        <v>2351</v>
+        <v>0</v>
       </c>
       <c r="Q12" s="3">
         <v>0</v>
@@ -3391,10 +3357,10 @@
         <v>0</v>
       </c>
       <c r="AD12" s="3">
-        <v>0</v>
+        <v>7439</v>
       </c>
       <c r="AE12" s="3">
-        <v>7439</v>
+        <v>0</v>
       </c>
       <c r="AF12" s="3">
         <v>0</v>
@@ -3411,20 +3377,17 @@
       <c r="AJ12" s="3">
         <v>0</v>
       </c>
-      <c r="AK12" s="3">
-        <v>0</v>
-      </c>
     </row>
-    <row r="13" spans="1:37" ht="17" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:36" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C13" s="7" t="s">
+      <c r="B13" s="7" t="s">
         <v>83</v>
       </c>
+      <c r="C13" s="3">
+        <v>0</v>
+      </c>
       <c r="D13" s="3">
         <v>0</v>
       </c>
@@ -3450,17 +3413,17 @@
         <v>0</v>
       </c>
       <c r="L13" s="3">
-        <v>0</v>
+        <v>87</v>
       </c>
       <c r="M13" s="3">
-        <v>87</v>
-      </c>
-      <c r="N13" s="3">
-        <v>0</v>
-      </c>
-      <c r="O13" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="N13" s="3" t="s">
         <v>1</v>
       </c>
+      <c r="O13" s="3">
+        <v>0</v>
+      </c>
       <c r="P13" s="3">
         <v>0</v>
       </c>
@@ -3498,10 +3461,10 @@
         <v>0</v>
       </c>
       <c r="AB13" s="3">
-        <v>0</v>
+        <v>126</v>
       </c>
       <c r="AC13" s="3">
-        <v>126</v>
+        <v>0</v>
       </c>
       <c r="AD13" s="3">
         <v>0</v>
@@ -3513,10 +3476,10 @@
         <v>0</v>
       </c>
       <c r="AG13" s="3">
-        <v>0</v>
+        <v>4068</v>
       </c>
       <c r="AH13" s="3">
-        <v>4068</v>
+        <v>0</v>
       </c>
       <c r="AI13" s="3">
         <v>0</v>
@@ -3524,20 +3487,17 @@
       <c r="AJ13" s="3">
         <v>0</v>
       </c>
-      <c r="AK13" s="3">
-        <v>0</v>
-      </c>
     </row>
-    <row r="14" spans="1:37" ht="17" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:36" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C14" s="7" t="s">
+      <c r="B14" s="7" t="s">
         <v>84</v>
       </c>
+      <c r="C14" s="3">
+        <v>0</v>
+      </c>
       <c r="D14" s="3">
         <v>0</v>
       </c>
@@ -3545,40 +3505,40 @@
         <v>0</v>
       </c>
       <c r="F14" s="3">
-        <v>0</v>
+        <v>1709</v>
       </c>
       <c r="G14" s="3">
-        <v>1709</v>
+        <v>0</v>
       </c>
       <c r="H14" s="3">
-        <v>0</v>
+        <v>8311</v>
       </c>
       <c r="I14" s="3">
-        <v>8311</v>
+        <v>0</v>
       </c>
       <c r="J14" s="3">
-        <v>0</v>
+        <v>10607</v>
       </c>
       <c r="K14" s="3">
-        <v>10607</v>
+        <v>0</v>
       </c>
       <c r="L14" s="3">
         <v>0</v>
       </c>
       <c r="M14" s="3">
-        <v>0</v>
+        <v>3957</v>
       </c>
       <c r="N14" s="3">
-        <v>3957</v>
-      </c>
-      <c r="O14" s="3">
-        <v>0</v>
-      </c>
-      <c r="P14" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="O14" s="3" t="s">
         <v>1</v>
       </c>
+      <c r="P14" s="3">
+        <v>6889</v>
+      </c>
       <c r="Q14" s="3">
-        <v>6889</v>
+        <v>0</v>
       </c>
       <c r="R14" s="3">
         <v>0</v>
@@ -3590,10 +3550,10 @@
         <v>0</v>
       </c>
       <c r="U14" s="3">
-        <v>0</v>
+        <v>11808</v>
       </c>
       <c r="V14" s="3">
-        <v>11808</v>
+        <v>0</v>
       </c>
       <c r="W14" s="3">
         <v>0</v>
@@ -3637,20 +3597,17 @@
       <c r="AJ14" s="3">
         <v>0</v>
       </c>
-      <c r="AK14" s="3">
-        <v>0</v>
-      </c>
     </row>
-    <row r="15" spans="1:37" ht="17" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:36" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C15" s="7" t="s">
+      <c r="B15" s="7" t="s">
         <v>68</v>
       </c>
+      <c r="C15" s="3">
+        <v>0</v>
+      </c>
       <c r="D15" s="3">
         <v>0</v>
       </c>
@@ -3685,14 +3642,14 @@
         <v>0</v>
       </c>
       <c r="O15" s="3">
-        <v>0</v>
-      </c>
-      <c r="P15" s="3">
         <v>3358</v>
       </c>
-      <c r="Q15" s="3" t="s">
+      <c r="P15" s="3" t="s">
         <v>1</v>
       </c>
+      <c r="Q15" s="3">
+        <v>0</v>
+      </c>
       <c r="R15" s="3">
         <v>0</v>
       </c>
@@ -3700,10 +3657,10 @@
         <v>0</v>
       </c>
       <c r="T15" s="3">
-        <v>0</v>
+        <v>1992</v>
       </c>
       <c r="U15" s="3">
-        <v>1992</v>
+        <v>0</v>
       </c>
       <c r="V15" s="3">
         <v>0</v>
@@ -3750,22 +3707,19 @@
       <c r="AJ15" s="3">
         <v>0</v>
       </c>
-      <c r="AK15" s="3">
-        <v>0</v>
-      </c>
     </row>
-    <row r="16" spans="1:37" ht="17" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:36" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C16" s="7" t="s">
+      <c r="B16" s="7" t="s">
         <v>85</v>
       </c>
+      <c r="C16" s="3">
+        <v>1061</v>
+      </c>
       <c r="D16" s="3">
-        <v>1061</v>
+        <v>0</v>
       </c>
       <c r="E16" s="3">
         <v>0</v>
@@ -3803,12 +3757,12 @@
       <c r="P16" s="3">
         <v>0</v>
       </c>
-      <c r="Q16" s="3">
-        <v>0</v>
-      </c>
-      <c r="R16" s="3" t="s">
+      <c r="Q16" s="3" t="s">
         <v>1</v>
       </c>
+      <c r="R16" s="3">
+        <v>0</v>
+      </c>
       <c r="S16" s="3">
         <v>0</v>
       </c>
@@ -3816,10 +3770,10 @@
         <v>0</v>
       </c>
       <c r="U16" s="3">
-        <v>0</v>
+        <v>2184</v>
       </c>
       <c r="V16" s="3">
-        <v>2184</v>
+        <v>0</v>
       </c>
       <c r="W16" s="3">
         <v>0</v>
@@ -3831,10 +3785,10 @@
         <v>0</v>
       </c>
       <c r="Z16" s="3">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="AA16" s="3">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="AB16" s="3">
         <v>0</v>
@@ -3863,28 +3817,25 @@
       <c r="AJ16" s="3">
         <v>0</v>
       </c>
-      <c r="AK16" s="3">
-        <v>0</v>
-      </c>
     </row>
-    <row r="17" spans="1:37" ht="17" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:36" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C17" s="7" t="s">
+      <c r="B17" s="7" t="s">
         <v>86</v>
       </c>
+      <c r="C17" s="3">
+        <v>0</v>
+      </c>
       <c r="D17" s="3">
         <v>0</v>
       </c>
       <c r="E17" s="3">
-        <v>0</v>
+        <v>974</v>
       </c>
       <c r="F17" s="3">
-        <v>974</v>
+        <v>0</v>
       </c>
       <c r="G17" s="3">
         <v>0</v>
@@ -3919,14 +3870,14 @@
       <c r="Q17" s="3">
         <v>0</v>
       </c>
-      <c r="R17" s="3">
-        <v>0</v>
-      </c>
-      <c r="S17" s="3" t="s">
+      <c r="R17" s="3" t="s">
         <v>1</v>
       </c>
+      <c r="S17" s="3">
+        <v>8</v>
+      </c>
       <c r="T17" s="3">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="U17" s="3">
         <v>0</v>
@@ -3968,33 +3919,30 @@
         <v>0</v>
       </c>
       <c r="AH17" s="3">
-        <v>0</v>
+        <v>5196</v>
       </c>
       <c r="AI17" s="3">
-        <v>5196</v>
+        <v>0</v>
       </c>
       <c r="AJ17" s="3">
         <v>0</v>
       </c>
-      <c r="AK17" s="3">
-        <v>0</v>
-      </c>
     </row>
-    <row r="18" spans="1:37" ht="17" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:36" ht="17" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B18" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C18" s="7" t="s">
+      <c r="B18" s="7" t="s">
         <v>87</v>
       </c>
+      <c r="C18" s="3">
+        <v>0</v>
+      </c>
       <c r="D18" s="3">
-        <v>0</v>
+        <v>240</v>
       </c>
       <c r="E18" s="3">
-        <v>240</v>
+        <v>0</v>
       </c>
       <c r="F18" s="3">
         <v>0</v>
@@ -4033,14 +3981,14 @@
         <v>0</v>
       </c>
       <c r="R18" s="3">
-        <v>0</v>
-      </c>
-      <c r="S18" s="3">
         <v>3310</v>
       </c>
-      <c r="T18" s="3" t="s">
+      <c r="S18" s="3" t="s">
         <v>1</v>
       </c>
+      <c r="T18" s="3">
+        <v>0</v>
+      </c>
       <c r="U18" s="3">
         <v>0</v>
       </c>
@@ -4072,13 +4020,13 @@
         <v>0</v>
       </c>
       <c r="AE18" s="3">
-        <v>0</v>
+        <v>307</v>
       </c>
       <c r="AF18" s="3">
-        <v>307</v>
+        <v>1365</v>
       </c>
       <c r="AG18" s="3">
-        <v>1365</v>
+        <v>0</v>
       </c>
       <c r="AH18" s="3">
         <v>0</v>
@@ -4089,20 +4037,17 @@
       <c r="AJ18" s="3">
         <v>0</v>
       </c>
-      <c r="AK18" s="3">
-        <v>0</v>
-      </c>
     </row>
-    <row r="19" spans="1:37" ht="17" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:36" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C19" s="7" t="s">
+      <c r="B19" s="7" t="s">
         <v>88</v>
       </c>
+      <c r="C19" s="3">
+        <v>0</v>
+      </c>
       <c r="D19" s="3">
         <v>0</v>
       </c>
@@ -4140,10 +4085,10 @@
         <v>0</v>
       </c>
       <c r="P19" s="3">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="Q19" s="3">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="R19" s="3">
         <v>0</v>
@@ -4151,12 +4096,12 @@
       <c r="S19" s="3">
         <v>0</v>
       </c>
-      <c r="T19" s="3">
-        <v>0</v>
-      </c>
-      <c r="U19" s="3" t="s">
+      <c r="T19" s="3" t="s">
         <v>1</v>
       </c>
+      <c r="U19" s="3">
+        <v>0</v>
+      </c>
       <c r="V19" s="3">
         <v>0</v>
       </c>
@@ -4202,20 +4147,17 @@
       <c r="AJ19" s="3">
         <v>0</v>
       </c>
-      <c r="AK19" s="3">
-        <v>0</v>
-      </c>
     </row>
-    <row r="20" spans="1:37" ht="17" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:36" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B20" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C20" s="7" t="s">
+      <c r="B20" s="7" t="s">
         <v>89</v>
       </c>
+      <c r="C20" s="3">
+        <v>0</v>
+      </c>
       <c r="D20" s="3">
         <v>0</v>
       </c>
@@ -4229,10 +4171,10 @@
         <v>0</v>
       </c>
       <c r="H20" s="3">
-        <v>0</v>
+        <v>510</v>
       </c>
       <c r="I20" s="3">
-        <v>510</v>
+        <v>0</v>
       </c>
       <c r="J20" s="3">
         <v>0</v>
@@ -4250,16 +4192,16 @@
         <v>0</v>
       </c>
       <c r="O20" s="3">
-        <v>0</v>
+        <v>1215</v>
       </c>
       <c r="P20" s="3">
-        <v>1215</v>
+        <v>0</v>
       </c>
       <c r="Q20" s="3">
-        <v>0</v>
+        <v>314</v>
       </c>
       <c r="R20" s="3">
-        <v>314</v>
+        <v>0</v>
       </c>
       <c r="S20" s="3">
         <v>0</v>
@@ -4267,12 +4209,12 @@
       <c r="T20" s="3">
         <v>0</v>
       </c>
-      <c r="U20" s="3">
-        <v>0</v>
-      </c>
-      <c r="V20" s="3" t="s">
+      <c r="U20" s="3" t="s">
         <v>1</v>
       </c>
+      <c r="V20" s="3">
+        <v>0</v>
+      </c>
       <c r="W20" s="3">
         <v>0</v>
       </c>
@@ -4307,28 +4249,25 @@
         <v>0</v>
       </c>
       <c r="AH20" s="3">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="AI20" s="3">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="AJ20" s="3">
         <v>0</v>
       </c>
-      <c r="AK20" s="3">
-        <v>0</v>
-      </c>
     </row>
-    <row r="21" spans="1:37" ht="17" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:36" ht="17" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B21" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C21" s="7" t="s">
+      <c r="B21" s="7" t="s">
         <v>90</v>
       </c>
+      <c r="C21" s="3">
+        <v>0</v>
+      </c>
       <c r="D21" s="3">
         <v>0</v>
       </c>
@@ -4383,17 +4322,17 @@
       <c r="U21" s="3">
         <v>0</v>
       </c>
-      <c r="V21" s="3">
-        <v>0</v>
-      </c>
-      <c r="W21" s="3" t="s">
+      <c r="V21" s="3" t="s">
         <v>1</v>
       </c>
+      <c r="W21" s="3">
+        <v>0</v>
+      </c>
       <c r="X21" s="3">
-        <v>0</v>
+        <v>3066</v>
       </c>
       <c r="Y21" s="3">
-        <v>3066</v>
+        <v>0</v>
       </c>
       <c r="Z21" s="3">
         <v>0</v>
@@ -4428,20 +4367,17 @@
       <c r="AJ21" s="3">
         <v>0</v>
       </c>
-      <c r="AK21" s="3">
-        <v>0</v>
-      </c>
     </row>
-    <row r="22" spans="1:37" ht="17" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:36" ht="17" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B22" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C22" s="7" t="s">
+      <c r="B22" s="7" t="s">
         <v>91</v>
       </c>
+      <c r="C22" s="3">
+        <v>0</v>
+      </c>
       <c r="D22" s="3">
         <v>0</v>
       </c>
@@ -4449,10 +4385,10 @@
         <v>0</v>
       </c>
       <c r="F22" s="3">
-        <v>0</v>
+        <v>1868</v>
       </c>
       <c r="G22" s="3">
-        <v>1868</v>
+        <v>0</v>
       </c>
       <c r="H22" s="3">
         <v>0</v>
@@ -4461,10 +4397,10 @@
         <v>0</v>
       </c>
       <c r="J22" s="3">
-        <v>0</v>
+        <v>728</v>
       </c>
       <c r="K22" s="3">
-        <v>728</v>
+        <v>0</v>
       </c>
       <c r="L22" s="3">
         <v>0</v>
@@ -4499,12 +4435,12 @@
       <c r="V22" s="3">
         <v>0</v>
       </c>
-      <c r="W22" s="3">
-        <v>0</v>
-      </c>
-      <c r="X22" s="3" t="s">
+      <c r="W22" s="3" t="s">
         <v>1</v>
       </c>
+      <c r="X22" s="3">
+        <v>0</v>
+      </c>
       <c r="Y22" s="3">
         <v>0</v>
       </c>
@@ -4541,20 +4477,17 @@
       <c r="AJ22" s="3">
         <v>0</v>
       </c>
-      <c r="AK22" s="3">
-        <v>0</v>
-      </c>
     </row>
-    <row r="23" spans="1:37" ht="17" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:36" ht="17" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B23" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C23" s="7" t="s">
+      <c r="B23" s="7" t="s">
         <v>92</v>
       </c>
+      <c r="C23" s="3">
+        <v>0</v>
+      </c>
       <c r="D23" s="3">
         <v>0</v>
       </c>
@@ -4580,10 +4513,10 @@
         <v>0</v>
       </c>
       <c r="L23" s="3">
-        <v>0</v>
+        <v>497</v>
       </c>
       <c r="M23" s="3">
-        <v>497</v>
+        <v>0</v>
       </c>
       <c r="N23" s="3">
         <v>0</v>
@@ -4610,17 +4543,17 @@
         <v>0</v>
       </c>
       <c r="V23" s="3">
-        <v>0</v>
+        <v>1495</v>
       </c>
       <c r="W23" s="3">
-        <v>1495</v>
-      </c>
-      <c r="X23" s="3">
-        <v>0</v>
-      </c>
-      <c r="Y23" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="X23" s="3" t="s">
         <v>1</v>
       </c>
+      <c r="Y23" s="3">
+        <v>0</v>
+      </c>
       <c r="Z23" s="3">
         <v>0</v>
       </c>
@@ -4654,28 +4587,25 @@
       <c r="AJ23" s="3">
         <v>0</v>
       </c>
-      <c r="AK23" s="3">
-        <v>0</v>
-      </c>
     </row>
-    <row r="24" spans="1:37" ht="17" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:36" ht="17" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B24" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C24" s="7" t="s">
+      <c r="B24" s="7" t="s">
         <v>93</v>
       </c>
+      <c r="C24" s="3">
+        <v>614</v>
+      </c>
       <c r="D24" s="3">
-        <v>614</v>
+        <v>0</v>
       </c>
       <c r="E24" s="3">
-        <v>0</v>
+        <v>294</v>
       </c>
       <c r="F24" s="3">
-        <v>294</v>
+        <v>0</v>
       </c>
       <c r="G24" s="3">
         <v>0</v>
@@ -4731,12 +4661,12 @@
       <c r="X24" s="3">
         <v>0</v>
       </c>
-      <c r="Y24" s="3">
-        <v>0</v>
-      </c>
-      <c r="Z24" s="3" t="s">
+      <c r="Y24" s="3" t="s">
         <v>1</v>
       </c>
+      <c r="Z24" s="3">
+        <v>0</v>
+      </c>
       <c r="AA24" s="3">
         <v>0</v>
       </c>
@@ -4753,10 +4683,10 @@
         <v>0</v>
       </c>
       <c r="AF24" s="3">
-        <v>0</v>
+        <v>893</v>
       </c>
       <c r="AG24" s="3">
-        <v>893</v>
+        <v>0</v>
       </c>
       <c r="AH24" s="3">
         <v>0</v>
@@ -4767,20 +4697,17 @@
       <c r="AJ24" s="3">
         <v>0</v>
       </c>
-      <c r="AK24" s="3">
-        <v>0</v>
-      </c>
     </row>
-    <row r="25" spans="1:37" ht="17" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:36" ht="17" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B25" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C25" s="7" t="s">
+      <c r="B25" s="7" t="s">
         <v>94</v>
       </c>
+      <c r="C25" s="3">
+        <v>0</v>
+      </c>
       <c r="D25" s="3">
         <v>0</v>
       </c>
@@ -4821,10 +4748,10 @@
         <v>0</v>
       </c>
       <c r="Q25" s="3">
-        <v>0</v>
+        <v>3811</v>
       </c>
       <c r="R25" s="3">
-        <v>3811</v>
+        <v>0</v>
       </c>
       <c r="S25" s="3">
         <v>0</v>
@@ -4847,12 +4774,12 @@
       <c r="Y25" s="3">
         <v>0</v>
       </c>
-      <c r="Z25" s="3">
-        <v>0</v>
-      </c>
-      <c r="AA25" s="3" t="s">
+      <c r="Z25" s="3" t="s">
         <v>1</v>
       </c>
+      <c r="AA25" s="3">
+        <v>0</v>
+      </c>
       <c r="AB25" s="3">
         <v>0</v>
       </c>
@@ -4866,10 +4793,10 @@
         <v>0</v>
       </c>
       <c r="AF25" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AG25" s="3">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AH25" s="3">
         <v>0</v>
@@ -4880,20 +4807,17 @@
       <c r="AJ25" s="3">
         <v>0</v>
       </c>
-      <c r="AK25" s="3">
-        <v>0</v>
-      </c>
     </row>
-    <row r="26" spans="1:37" ht="17" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:36" ht="17" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B26" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C26" s="7" t="s">
+      <c r="B26" s="7" t="s">
         <v>95</v>
       </c>
+      <c r="C26" s="3">
+        <v>0</v>
+      </c>
       <c r="D26" s="3">
         <v>0</v>
       </c>
@@ -4901,10 +4825,10 @@
         <v>0</v>
       </c>
       <c r="F26" s="3">
-        <v>0</v>
+        <v>5789</v>
       </c>
       <c r="G26" s="3">
-        <v>5789</v>
+        <v>0</v>
       </c>
       <c r="H26" s="3">
         <v>0</v>
@@ -4913,10 +4837,10 @@
         <v>0</v>
       </c>
       <c r="J26" s="3">
-        <v>0</v>
+        <v>3510</v>
       </c>
       <c r="K26" s="3">
-        <v>3510</v>
+        <v>0</v>
       </c>
       <c r="L26" s="3">
         <v>0</v>
@@ -4963,14 +4887,14 @@
       <c r="Z26" s="3">
         <v>0</v>
       </c>
-      <c r="AA26" s="3">
-        <v>0</v>
-      </c>
-      <c r="AB26" s="3" t="s">
+      <c r="AA26" s="3" t="s">
         <v>1</v>
       </c>
+      <c r="AB26" s="3">
+        <v>1257</v>
+      </c>
       <c r="AC26" s="3">
-        <v>1257</v>
+        <v>0</v>
       </c>
       <c r="AD26" s="3">
         <v>0</v>
@@ -4993,20 +4917,17 @@
       <c r="AJ26" s="3">
         <v>0</v>
       </c>
-      <c r="AK26" s="3">
-        <v>0</v>
-      </c>
     </row>
-    <row r="27" spans="1:37" ht="17" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:36" ht="17" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B27" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C27" s="7" t="s">
+      <c r="B27" s="7" t="s">
         <v>96</v>
       </c>
+      <c r="C27" s="3">
+        <v>0</v>
+      </c>
       <c r="D27" s="3">
         <v>0</v>
       </c>
@@ -5029,19 +4950,19 @@
         <v>0</v>
       </c>
       <c r="K27" s="3">
-        <v>0</v>
+        <v>3828</v>
       </c>
       <c r="L27" s="3">
-        <v>3828</v>
+        <v>0</v>
       </c>
       <c r="M27" s="3">
         <v>0</v>
       </c>
       <c r="N27" s="3">
-        <v>0</v>
+        <v>111</v>
       </c>
       <c r="O27" s="3">
-        <v>111</v>
+        <v>0</v>
       </c>
       <c r="P27" s="3">
         <v>0</v>
@@ -5077,14 +4998,14 @@
         <v>0</v>
       </c>
       <c r="AA27" s="3">
-        <v>0</v>
-      </c>
-      <c r="AB27" s="3">
         <v>2814</v>
       </c>
-      <c r="AC27" s="3" t="s">
+      <c r="AB27" s="3" t="s">
         <v>1</v>
       </c>
+      <c r="AC27" s="3">
+        <v>0</v>
+      </c>
       <c r="AD27" s="3">
         <v>0</v>
       </c>
@@ -5095,10 +5016,10 @@
         <v>0</v>
       </c>
       <c r="AG27" s="3">
-        <v>0</v>
+        <v>7764</v>
       </c>
       <c r="AH27" s="3">
-        <v>7764</v>
+        <v>0</v>
       </c>
       <c r="AI27" s="3">
         <v>0</v>
@@ -5106,20 +5027,17 @@
       <c r="AJ27" s="3">
         <v>0</v>
       </c>
-      <c r="AK27" s="3">
-        <v>0</v>
-      </c>
     </row>
-    <row r="28" spans="1:37" ht="17" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:36" ht="17" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B28" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C28" s="7" t="s">
+      <c r="B28" s="7" t="s">
         <v>97</v>
       </c>
+      <c r="C28" s="3">
+        <v>0</v>
+      </c>
       <c r="D28" s="3">
         <v>0</v>
       </c>
@@ -5136,13 +5054,13 @@
         <v>0</v>
       </c>
       <c r="I28" s="3">
-        <v>0</v>
+        <v>6866</v>
       </c>
       <c r="J28" s="3">
-        <v>6866</v>
+        <v>135</v>
       </c>
       <c r="K28" s="3">
-        <v>135</v>
+        <v>0</v>
       </c>
       <c r="L28" s="3">
         <v>0</v>
@@ -5195,12 +5113,12 @@
       <c r="AB28" s="3">
         <v>0</v>
       </c>
-      <c r="AC28" s="3">
-        <v>0</v>
-      </c>
-      <c r="AD28" s="3" t="s">
+      <c r="AC28" s="3" t="s">
         <v>1</v>
       </c>
+      <c r="AD28" s="3">
+        <v>0</v>
+      </c>
       <c r="AE28" s="3">
         <v>0</v>
       </c>
@@ -5208,31 +5126,28 @@
         <v>0</v>
       </c>
       <c r="AG28" s="3">
-        <v>0</v>
+        <v>254</v>
       </c>
       <c r="AH28" s="3">
-        <v>254</v>
+        <v>0</v>
       </c>
       <c r="AI28" s="3">
-        <v>0</v>
+        <v>2338</v>
       </c>
       <c r="AJ28" s="3">
-        <v>2338</v>
-      </c>
-      <c r="AK28" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:37" ht="17" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:36" ht="17" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B29" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C29" s="7" t="s">
+      <c r="B29" s="7" t="s">
         <v>98</v>
       </c>
+      <c r="C29" s="3">
+        <v>0</v>
+      </c>
       <c r="D29" s="3">
         <v>0</v>
       </c>
@@ -5261,10 +5176,10 @@
         <v>0</v>
       </c>
       <c r="M29" s="3">
-        <v>0</v>
+        <v>2819</v>
       </c>
       <c r="N29" s="3">
-        <v>2819</v>
+        <v>0</v>
       </c>
       <c r="O29" s="3">
         <v>0</v>
@@ -5311,12 +5226,12 @@
       <c r="AC29" s="3">
         <v>0</v>
       </c>
-      <c r="AD29" s="3">
-        <v>0</v>
-      </c>
-      <c r="AE29" s="3" t="s">
+      <c r="AD29" s="3" t="s">
         <v>1</v>
       </c>
+      <c r="AE29" s="3">
+        <v>0</v>
+      </c>
       <c r="AF29" s="3">
         <v>0</v>
       </c>
@@ -5332,20 +5247,17 @@
       <c r="AJ29" s="3">
         <v>0</v>
       </c>
-      <c r="AK29" s="3">
-        <v>0</v>
-      </c>
     </row>
-    <row r="30" spans="1:37" ht="17" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:36" ht="17" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B30" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C30" s="7" t="s">
+      <c r="B30" s="7" t="s">
         <v>99</v>
       </c>
+      <c r="C30" s="3">
+        <v>0</v>
+      </c>
       <c r="D30" s="3">
         <v>0</v>
       </c>
@@ -5356,10 +5268,10 @@
         <v>0</v>
       </c>
       <c r="G30" s="3">
-        <v>0</v>
+        <v>2618</v>
       </c>
       <c r="H30" s="3">
-        <v>2618</v>
+        <v>0</v>
       </c>
       <c r="I30" s="3">
         <v>0</v>
@@ -5392,10 +5304,10 @@
         <v>0</v>
       </c>
       <c r="S30" s="3">
-        <v>0</v>
+        <v>587</v>
       </c>
       <c r="T30" s="3">
-        <v>587</v>
+        <v>0</v>
       </c>
       <c r="U30" s="3">
         <v>0</v>
@@ -5427,14 +5339,14 @@
       <c r="AD30" s="3">
         <v>0</v>
       </c>
-      <c r="AE30" s="3">
-        <v>0</v>
-      </c>
-      <c r="AF30" s="3" t="s">
+      <c r="AE30" s="3" t="s">
         <v>1</v>
       </c>
+      <c r="AF30" s="3">
+        <v>1648</v>
+      </c>
       <c r="AG30" s="3">
-        <v>1648</v>
+        <v>0</v>
       </c>
       <c r="AH30" s="3">
         <v>0</v>
@@ -5445,34 +5357,31 @@
       <c r="AJ30" s="3">
         <v>0</v>
       </c>
-      <c r="AK30" s="3">
-        <v>0</v>
-      </c>
     </row>
-    <row r="31" spans="1:37" ht="17" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:36" ht="17" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B31" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C31" s="7" t="s">
+      <c r="B31" s="7" t="s">
         <v>100</v>
       </c>
+      <c r="C31" s="3">
+        <v>103</v>
+      </c>
       <c r="D31" s="3">
-        <v>103</v>
+        <v>0</v>
       </c>
       <c r="E31" s="3">
-        <v>0</v>
+        <v>1571</v>
       </c>
       <c r="F31" s="3">
-        <v>1571</v>
+        <v>0</v>
       </c>
       <c r="G31" s="3">
-        <v>0</v>
+        <v>46</v>
       </c>
       <c r="H31" s="3">
-        <v>46</v>
+        <v>0</v>
       </c>
       <c r="I31" s="3">
         <v>0</v>
@@ -5502,13 +5411,13 @@
         <v>0</v>
       </c>
       <c r="R31" s="3">
-        <v>0</v>
+        <v>1707</v>
       </c>
       <c r="S31" s="3">
-        <v>1707</v>
+        <v>75</v>
       </c>
       <c r="T31" s="3">
-        <v>75</v>
+        <v>0</v>
       </c>
       <c r="U31" s="3">
         <v>0</v>
@@ -5523,13 +5432,13 @@
         <v>0</v>
       </c>
       <c r="Y31" s="3">
-        <v>0</v>
+        <v>852</v>
       </c>
       <c r="Z31" s="3">
-        <v>852</v>
+        <v>2330</v>
       </c>
       <c r="AA31" s="3">
-        <v>2330</v>
+        <v>0</v>
       </c>
       <c r="AB31" s="3">
         <v>0</v>
@@ -5541,14 +5450,14 @@
         <v>0</v>
       </c>
       <c r="AE31" s="3">
-        <v>0</v>
-      </c>
-      <c r="AF31" s="3">
         <v>55</v>
       </c>
-      <c r="AG31" s="3" t="s">
+      <c r="AF31" s="3" t="s">
         <v>1</v>
       </c>
+      <c r="AG31" s="3">
+        <v>0</v>
+      </c>
       <c r="AH31" s="3">
         <v>0</v>
       </c>
@@ -5558,20 +5467,17 @@
       <c r="AJ31" s="3">
         <v>0</v>
       </c>
-      <c r="AK31" s="3">
-        <v>0</v>
-      </c>
     </row>
-    <row r="32" spans="1:37" ht="17" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:36" ht="17" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B32" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C32" s="7" t="s">
+      <c r="B32" s="7" t="s">
         <v>101</v>
       </c>
+      <c r="C32" s="3">
+        <v>0</v>
+      </c>
       <c r="D32" s="3">
         <v>0</v>
       </c>
@@ -5591,22 +5497,22 @@
         <v>0</v>
       </c>
       <c r="J32" s="3">
-        <v>0</v>
+        <v>949</v>
       </c>
       <c r="K32" s="3">
-        <v>949</v>
+        <v>3838</v>
       </c>
       <c r="L32" s="3">
-        <v>3838</v>
+        <v>0</v>
       </c>
       <c r="M32" s="3">
         <v>0</v>
       </c>
       <c r="N32" s="3">
-        <v>0</v>
+        <v>2882</v>
       </c>
       <c r="O32" s="3">
-        <v>2882</v>
+        <v>0</v>
       </c>
       <c r="P32" s="3">
         <v>0</v>
@@ -5645,13 +5551,13 @@
         <v>0</v>
       </c>
       <c r="AB32" s="3">
-        <v>0</v>
+        <v>2633</v>
       </c>
       <c r="AC32" s="3">
-        <v>2633</v>
+        <v>1394</v>
       </c>
       <c r="AD32" s="3">
-        <v>1394</v>
+        <v>0</v>
       </c>
       <c r="AE32" s="3">
         <v>0</v>
@@ -5659,37 +5565,34 @@
       <c r="AF32" s="3">
         <v>0</v>
       </c>
-      <c r="AG32" s="3">
-        <v>0</v>
-      </c>
-      <c r="AH32" s="3" t="s">
+      <c r="AG32" s="3" t="s">
         <v>1</v>
       </c>
+      <c r="AH32" s="3">
+        <v>0</v>
+      </c>
       <c r="AI32" s="3">
         <v>0</v>
       </c>
       <c r="AJ32" s="3">
         <v>0</v>
       </c>
-      <c r="AK32" s="3">
-        <v>0</v>
-      </c>
     </row>
-    <row r="33" spans="1:37" ht="17" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:36" ht="17" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B33" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C33" s="7" t="s">
+      <c r="B33" s="7" t="s">
         <v>102</v>
       </c>
+      <c r="C33" s="3">
+        <v>0</v>
+      </c>
       <c r="D33" s="3">
-        <v>0</v>
+        <v>470</v>
       </c>
       <c r="E33" s="3">
-        <v>470</v>
+        <v>0</v>
       </c>
       <c r="F33" s="3">
         <v>0</v>
@@ -5728,19 +5631,19 @@
         <v>0</v>
       </c>
       <c r="R33" s="3">
-        <v>0</v>
+        <v>3574</v>
       </c>
       <c r="S33" s="3">
-        <v>3574</v>
+        <v>0</v>
       </c>
       <c r="T33" s="3">
         <v>0</v>
       </c>
       <c r="U33" s="3">
-        <v>0</v>
+        <v>6799</v>
       </c>
       <c r="V33" s="3">
-        <v>6799</v>
+        <v>0</v>
       </c>
       <c r="W33" s="3">
         <v>0</v>
@@ -5775,29 +5678,26 @@
       <c r="AG33" s="3">
         <v>0</v>
       </c>
-      <c r="AH33" s="3">
-        <v>0</v>
-      </c>
-      <c r="AI33" s="3" t="s">
+      <c r="AH33" s="3" t="s">
         <v>1</v>
       </c>
+      <c r="AI33" s="3">
+        <v>0</v>
+      </c>
       <c r="AJ33" s="3">
         <v>0</v>
       </c>
-      <c r="AK33" s="3">
-        <v>0</v>
-      </c>
     </row>
-    <row r="34" spans="1:37" ht="17" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:36" ht="17" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B34" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="C34" s="7" t="s">
+      <c r="B34" s="7" t="s">
         <v>103</v>
       </c>
+      <c r="C34" s="3">
+        <v>0</v>
+      </c>
       <c r="D34" s="3">
         <v>0</v>
       </c>
@@ -5814,10 +5714,10 @@
         <v>0</v>
       </c>
       <c r="I34" s="3">
-        <v>0</v>
+        <v>141</v>
       </c>
       <c r="J34" s="3">
-        <v>141</v>
+        <v>0</v>
       </c>
       <c r="K34" s="3">
         <v>0</v>
@@ -5844,10 +5744,10 @@
         <v>0</v>
       </c>
       <c r="S34" s="3">
-        <v>0</v>
+        <v>6000</v>
       </c>
       <c r="T34" s="3">
-        <v>6000</v>
+        <v>0</v>
       </c>
       <c r="U34" s="3">
         <v>0</v>
@@ -5874,10 +5774,10 @@
         <v>0</v>
       </c>
       <c r="AC34" s="3">
-        <v>0</v>
+        <v>64</v>
       </c>
       <c r="AD34" s="3">
-        <v>64</v>
+        <v>0</v>
       </c>
       <c r="AE34" s="3">
         <v>0</v>
@@ -5891,26 +5791,23 @@
       <c r="AH34" s="3">
         <v>0</v>
       </c>
-      <c r="AI34" s="3">
-        <v>0</v>
-      </c>
-      <c r="AJ34" s="3" t="s">
+      <c r="AI34" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="AK34" s="3">
+      <c r="AJ34" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:37" ht="17" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:36" ht="17" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B35" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C35" s="7" t="s">
+      <c r="B35" s="7" t="s">
         <v>104</v>
       </c>
+      <c r="C35" s="3">
+        <v>0</v>
+      </c>
       <c r="D35" s="3">
         <v>0</v>
       </c>
@@ -6007,10 +5904,7 @@
       <c r="AI35" s="3">
         <v>0</v>
       </c>
-      <c r="AJ35" s="3">
-        <v>0</v>
-      </c>
-      <c r="AK35" s="3" t="s">
+      <c r="AJ35" s="3" t="s">
         <v>1</v>
       </c>
     </row>
@@ -9918,7 +9812,7 @@
   <dimension ref="A1:AJ35"/>
   <sheetViews>
     <sheetView zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <selection activeCell="M45" sqref="M45"/>
+      <selection activeCell="N40" sqref="N40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="7.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -13368,7 +13262,9 @@
       <c r="F32" s="1">
         <v>0</v>
       </c>
-      <c r="G32" s="1"/>
+      <c r="G32" s="1">
+        <v>0</v>
+      </c>
       <c r="H32" s="1">
         <v>0</v>
       </c>
@@ -13476,7 +13372,9 @@
       <c r="F33" s="1">
         <v>0</v>
       </c>
-      <c r="G33" s="1"/>
+      <c r="G33" s="1">
+        <v>0</v>
+      </c>
       <c r="H33" s="1">
         <v>0</v>
       </c>
@@ -13584,7 +13482,9 @@
       <c r="F34" s="1">
         <v>0</v>
       </c>
-      <c r="G34" s="1"/>
+      <c r="G34" s="1">
+        <v>0</v>
+      </c>
       <c r="H34" s="1">
         <v>0</v>
       </c>

</xml_diff>